<commit_message>
Add vConsump to eDC_BalanceP for storage units
Disable H2
Disable Invest for storage units
</commit_message>
<xml_diff>
--- a/data/example/Global_Parameters.xlsx
+++ b/data/example/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F49237-190B-4751-8EFB-3E53A17AC70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CD2E4B-680D-4FAA-9284-B3CC66F5ADD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34572" yWindow="-17508" windowWidth="30936" windowHeight="16776" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>[h]</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Solve LEGO as relaxed mixed integer problem (Yes: Commitment of thermal power plants between 1 and 0; No: Commitment either 1 or 0)</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -848,7 +851,9 @@
   </sheetPr>
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -998,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>10</v>
@@ -1233,18 +1238,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1394,6 +1399,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1405,14 +1418,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed pEnableRMIP to be converted to bool
Add Excel printer
</commit_message>
<xml_diff>
--- a/data/example/Global_Parameters.xlsx
+++ b/data/example/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CD2E4B-680D-4FAA-9284-B3CC66F5ADD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080AD4E4-EB9D-4425-BCD2-7CA1A29700B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34572" yWindow="-17508" windowWidth="30936" windowHeight="16776" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42080" yWindow="890" windowWidth="19200" windowHeight="10160" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -423,12 +423,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Bad" xfId="8" builtinId="27"/>
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="8" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
@@ -851,29 +851,29 @@
   </sheetPr>
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.3984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="43" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1"/>
+    <col min="3" max="3" width="30.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" style="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="139.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="1"/>
+    <col min="6" max="6" width="139.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.265625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
@@ -893,7 +893,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
@@ -902,7 +902,7 @@
       </c>
       <c r="H4" s="17"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
@@ -916,13 +916,13 @@
       <c r="G5" s="11"/>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
@@ -934,7 +934,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
@@ -948,13 +948,13 @@
       <c r="G8" s="11"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="19"/>
     </row>
-    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -966,7 +966,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
@@ -980,13 +980,13 @@
       <c r="G11" s="11"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
@@ -998,7 +998,7 @@
       <c r="G13" s="11"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1018,13 +1018,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
@@ -1033,7 +1033,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
@@ -1065,13 +1065,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="7" t="s">
         <v>21</v>
       </c>
@@ -1080,7 +1080,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1092,7 +1092,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
@@ -1110,13 +1110,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="18"/>
     </row>
-    <row r="24" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="7" t="s">
         <v>6</v>
       </c>
@@ -1125,7 +1125,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1137,7 +1137,7 @@
       <c r="G25" s="11"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
@@ -1238,21 +1238,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1398,15 +1389,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1422,7 +1414,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1438,4 +1430,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Clean Global_Parameters and add option to select solver
</commit_message>
<xml_diff>
--- a/data/example/Global_Parameters.xlsx
+++ b/data/example/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CD2E4B-680D-4FAA-9284-B3CC66F5ADD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B97E30-EBBA-4B05-A050-BF8FC9BC25EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34572" yWindow="-17508" windowWidth="30936" windowHeight="16776" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>[h]</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>pEnableH2</t>
-  </si>
-  <si>
     <t>Short description</t>
   </si>
   <si>
@@ -96,30 +93,9 @@
     <t>Yes/No</t>
   </si>
   <si>
-    <t>Enable H2 sector</t>
-  </si>
-  <si>
-    <t>Enable H2 sector (electrolyzers)</t>
-  </si>
-  <si>
     <t>rMIP [Yes] or MIP [No]</t>
   </si>
   <si>
-    <t>pEnablePower</t>
-  </si>
-  <si>
-    <t>Enable Power Sector</t>
-  </si>
-  <si>
-    <t>Sectors</t>
-  </si>
-  <si>
-    <t>Enable Gas Sector</t>
-  </si>
-  <si>
-    <t>Enable Heat Sector</t>
-  </si>
-  <si>
     <t>Solver Options</t>
   </si>
   <si>
@@ -129,27 +105,9 @@
     <t>pEnableRMIP</t>
   </si>
   <si>
-    <t>Output Options</t>
-  </si>
-  <si>
     <t>[Yes, No]</t>
   </si>
   <si>
-    <t>[1=all, 2=reduced, 3=bare minimum]</t>
-  </si>
-  <si>
-    <t>pOutput</t>
-  </si>
-  <si>
-    <t>Granularity of output</t>
-  </si>
-  <si>
-    <t>pEnableGas</t>
-  </si>
-  <si>
-    <t>pEnableHeat</t>
-  </si>
-  <si>
     <t>Moving windows for LRP</t>
   </si>
   <si>
@@ -159,21 +117,9 @@
     <t>Parameters Global</t>
   </si>
   <si>
-    <t>Enable H2 Sector</t>
-  </si>
-  <si>
     <t>Source/ typical values</t>
   </si>
   <si>
-    <t>Currently not used</t>
-  </si>
-  <si>
-    <t>Set output level</t>
-  </si>
-  <si>
-    <t>1/2/3</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -183,14 +129,71 @@
     <t>Solve LEGO as relaxed mixed integer problem (Yes: Commitment of thermal power plants between 1 and 0; No: Commitment either 1 or 0)</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Solver selection</t>
+  </si>
+  <si>
+    <t>[name of requested solver]</t>
+  </si>
+  <si>
+    <t>pSolver</t>
+  </si>
+  <si>
+    <t>highs</t>
+  </si>
+  <si>
+    <t>Selected solver</t>
+  </si>
+  <si>
+    <t>Solver to use when solving the model</t>
+  </si>
+  <si>
+    <t>solver name</t>
+  </si>
+  <si>
+    <t>highs, gurobi, cplex, …</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>Power Scaling Factor</t>
+  </si>
+  <si>
+    <t>pPowerScalingFactor</t>
+  </si>
+  <si>
+    <t>[Scaling relative to 1MW]</t>
+  </si>
+  <si>
+    <t>MW scaling</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Cost Scaling Factor</t>
+  </si>
+  <si>
+    <t>pCostScalingFactor</t>
+  </si>
+  <si>
+    <t>[Scaling relative to 1€]</t>
+  </si>
+  <si>
+    <t>€ scaling</t>
+  </si>
+  <si>
+    <t>Scaling factor for €-values in input data (relative to 1€)</t>
+  </si>
+  <si>
+    <t>Scaling factor for power values in input data (relative to 1MW)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -267,19 +270,6 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -348,7 +338,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -359,9 +349,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -399,31 +388,20 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Bad" xfId="8" builtinId="27"/>
+  <cellStyles count="8">
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -433,35 +411,7 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <b/>
@@ -849,354 +799,256 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H31"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="5.640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="139.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.35546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>5</v>
-      </c>
       <c r="H3" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="18"/>
-    </row>
-    <row r="6" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="18"/>
-    </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="19"/>
-    </row>
-    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="E8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>33</v>
-      </c>
+    </row>
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="C12" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
+      <c r="G15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="9">
+        <v>168</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="18"/>
-    </row>
-    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="9">
-        <v>3</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="18"/>
-    </row>
-    <row r="26" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="9">
+      <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="13">
         <v>168</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="18">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C6">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1204,15 +1056,15 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1221,14 +1073,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C5:C6 C8:C9 C18 C11:C12 C14" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{13E44DF0-E318-4006-9E46-A03D51C3BE3C}">
-      <formula1>1</formula1>
-      <formula2>3</formula2>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C26" xr:uid="{B1F27E54-4BFD-2D4B-9633-37AF83A83F57}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C5 C12 C15" xr:uid="{13E44DF0-E318-4006-9E46-A03D51C3BE3C}"/>
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{B1F27E54-4BFD-2D4B-9633-37AF83A83F57}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Adjust cost-scaling to M€ for examples
Update to "merged" InOutModule
</commit_message>
<xml_diff>
--- a/data/example/Global_Parameters.xlsx
+++ b/data/example/Global_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B97E30-EBBA-4B05-A050-BF8FC9BC25EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451B080A-484F-47FB-9728-7071140E477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -977,7 +977,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="9">
-        <v>1E-3</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>38</v>
@@ -1048,27 +1048,27 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Enhance example files to force primitive storage usage
</commit_message>
<xml_diff>
--- a/data/example/Global_Parameters.xlsx
+++ b/data/example/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451B080A-484F-47FB-9728-7071140E477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D66E81-AB91-40EE-8EBC-573CD03393C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>[h]</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>General</t>
-  </si>
-  <si>
     <t>Moving window for LRP</t>
   </si>
   <si>
@@ -108,12 +105,6 @@
     <t>[Yes, No]</t>
   </si>
   <si>
-    <t>Moving windows for LRP</t>
-  </si>
-  <si>
-    <t>pMovWindow</t>
-  </si>
-  <si>
     <t>Parameters Global</t>
   </si>
   <si>
@@ -187,6 +178,42 @@
   </si>
   <si>
     <t>Scaling factor for power values in input data (relative to 1MW)</t>
+  </si>
+  <si>
+    <t>Long-Duration Storage</t>
+  </si>
+  <si>
+    <t>Moving windows for LRP (Long-Duration Storage)</t>
+  </si>
+  <si>
+    <t>pMovWindowLDS</t>
+  </si>
+  <si>
+    <t>Solve using Moving Window (with potential overlap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving windows length </t>
+  </si>
+  <si>
+    <t>pMovingWindowLength</t>
+  </si>
+  <si>
+    <t>Moving window length</t>
+  </si>
+  <si>
+    <t>Moving window length TODO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving windows overlap </t>
+  </si>
+  <si>
+    <t>pMovingWindowOverlap</t>
+  </si>
+  <si>
+    <t>Moving window overlap</t>
+  </si>
+  <si>
+    <t>Moving window overlap TODO</t>
   </si>
 </sst>
 </file>
@@ -411,7 +438,35 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -799,34 +854,36 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H19"/>
+  <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.35546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>2</v>
@@ -838,85 +895,85 @@
         <v>4</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="G5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="H5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="10"/>
       <c r="E10" s="10"/>
@@ -924,85 +981,85 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="9">
         <v>1E-3</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H12" s="13">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H15" s="13">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>0</v>
@@ -1011,52 +1068,138 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C19" s="9">
         <v>168</v>
       </c>
       <c r="E19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="H19" s="13">
         <v>168</v>
       </c>
     </row>
+    <row r="21" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="23" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="24" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1064,11 +1207,11 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+  <conditionalFormatting sqref="C26">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1096,12 +1239,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1247,6 +1384,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -1256,22 +1399,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1287,4 +1414,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add version specifier to Global_/Power_Parameters
Update to newest InOutModule with version checks for Parameter-Files
</commit_message>
<xml_diff>
--- a/data/example/Global_Parameters.xlsx
+++ b/data/example/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo2\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451B080A-484F-47FB-9728-7071140E477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD9B932-79A3-44F9-B21B-0DA8D023B87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33915" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>[h]</t>
   </si>
@@ -187,13 +187,19 @@
   </si>
   <si>
     <t>Scaling factor for power values in input data (relative to 1MW)</t>
+  </si>
+  <si>
+    <t>Format:</t>
+  </si>
+  <si>
+    <t>v0.1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -269,6 +275,11 @@
       <sz val="10"/>
       <name val="Aptos"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="8">
@@ -350,7 +361,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -399,6 +410,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -803,25 +820,33 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.35546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -841,7 +866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -853,7 +878,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -873,12 +898,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -889,7 +914,7 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -909,12 +934,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
@@ -924,7 +949,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
@@ -936,7 +961,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
@@ -956,12 +981,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
@@ -972,7 +997,7 @@
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
@@ -992,7 +1017,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -1000,7 +1025,7 @@
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1036,7 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1087,18 +1112,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1248,14 +1273,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1267,6 +1284,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Preparation for faster indexing variant SOCP
</commit_message>
<xml_diff>
--- a/data/example/Global_Parameters.xlsx
+++ b/data/example/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo2\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD9B932-79A3-44F9-B21B-0DA8D023B87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C97E64-C7E1-4847-B98D-92002217EFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33915" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="74060" yWindow="3380" windowWidth="28800" windowHeight="15240" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>pSolver</t>
   </si>
   <si>
-    <t>highs</t>
-  </si>
-  <si>
     <t>Selected solver</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>v0.1.0</t>
+  </si>
+  <si>
+    <t>gurobi</t>
   </si>
 </sst>
 </file>
@@ -419,11 +419,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
@@ -818,35 +818,37 @@
   </sheetPr>
   <dimension ref="B1:H19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="1"/>
+    <col min="6" max="6" width="120.86328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -866,7 +868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -878,32 +880,32 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -914,7 +916,7 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -934,14 +936,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10"/>
       <c r="E10" s="10"/>
@@ -949,75 +951,75 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="9">
         <v>1E-3</v>
       </c>
       <c r="E12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="H12" s="13">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="G15" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="13">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1027,7 @@
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1036,7 +1038,7 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1118,15 +1120,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1272,6 +1265,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
@@ -1289,14 +1291,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1312,4 +1306,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>